<commit_message>
bieu do tam xong
</commit_message>
<xml_diff>
--- a/PTUD_Nhom1/thongke.xlsx
+++ b/PTUD_Nhom1/thongke.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">Hóa đơn </t>
   </si>
@@ -35,61 +35,22 @@
     <t xml:space="preserve"> Lợi thuận</t>
   </si>
   <si>
-    <t>HD10871</t>
+    <t>HD002</t>
   </si>
   <si>
-    <t>KH89176</t>
-  </si>
-  <si>
-    <t>NV003</t>
-  </si>
-  <si>
-    <t>2024-04-17</t>
-  </si>
-  <si>
-    <t>2100.0</t>
-  </si>
-  <si>
-    <t>300.0</t>
-  </si>
-  <si>
-    <t>HD21497</t>
-  </si>
-  <si>
-    <t>KH94098</t>
-  </si>
-  <si>
-    <t>980.0</t>
-  </si>
-  <si>
-    <t>140.0</t>
-  </si>
-  <si>
-    <t>HD56595</t>
-  </si>
-  <si>
-    <t>KH08549</t>
+    <t>KH001</t>
   </si>
   <si>
     <t>NV001</t>
   </si>
   <si>
-    <t>2400.0</t>
+    <t>2024-02-23</t>
   </si>
   <si>
-    <t>480.0</t>
+    <t>2450000.0</t>
   </si>
   <si>
-    <t>HD69239</t>
-  </si>
-  <si>
-    <t>KH96175</t>
-  </si>
-  <si>
-    <t>940.0</t>
-  </si>
-  <si>
-    <t>180.0</t>
+    <t>728000.0</t>
   </si>
 </sst>
 </file>
@@ -134,7 +95,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -186,75 +147,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>